<commit_message>
feat: TOUR-1 allow updating of tour details
</commit_message>
<xml_diff>
--- a/Docs/Task List.xlsx
+++ b/Docs/Task List.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RJ\Documents\Projects\Personal\TourTheWorld\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79382F6-CEF3-42BF-AA38-ECF8DFF7368A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1253E1-4D78-4EF6-B3A5-38EB7DC5045F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Values" sheetId="2" r:id="rId2"/>
+    <sheet name="Screens" sheetId="3" r:id="rId2"/>
+    <sheet name="Values" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$290</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$307</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -131,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
   <si>
     <t>Task ID</t>
   </si>
@@ -253,9 +252,6 @@
     <t>Tour0009</t>
   </si>
   <si>
-    <t>As a user, I should be able to add tours</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -272,6 +268,126 @@
   </si>
   <si>
     <t>As a tour creator, I should be able to edit my tour's details</t>
+  </si>
+  <si>
+    <t>Tour0012</t>
+  </si>
+  <si>
+    <t>As a user, I should see my name instead of my email address in the header</t>
+  </si>
+  <si>
+    <t>Tour0013</t>
+  </si>
+  <si>
+    <t>As a user, I should be able to log in using my Facebook account</t>
+  </si>
+  <si>
+    <t>Tour0021</t>
+  </si>
+  <si>
+    <t>Tour0020</t>
+  </si>
+  <si>
+    <t>Tour0019</t>
+  </si>
+  <si>
+    <t>Tour0018</t>
+  </si>
+  <si>
+    <t>Tour0017</t>
+  </si>
+  <si>
+    <t>Tour0016</t>
+  </si>
+  <si>
+    <t>Tour0015</t>
+  </si>
+  <si>
+    <t>Tour0014</t>
+  </si>
+  <si>
+    <t>As a user, I should be able to set a profile picture which will be displayed beside my name in the header</t>
+  </si>
+  <si>
+    <t>After submitting new Tour details, prevent "Are you sure you want to leave?" pop-up from showing when navigating to another page</t>
+  </si>
+  <si>
+    <t>Add client-side global error handler</t>
+  </si>
+  <si>
+    <t>Add character counter to input fields with max length</t>
+  </si>
+  <si>
+    <t>As a tour creator, I should be able to add title and description to photos when adding tour photos</t>
+  </si>
+  <si>
+    <t>As a tour creator, I should be able to select a destination city/province</t>
+  </si>
+  <si>
+    <t>As a tour creator, I should be able to add contact details to my tour (e.g. phone #, FB/Messenger, E-Mail, Viber)</t>
+  </si>
+  <si>
+    <t>Tour0028</t>
+  </si>
+  <si>
+    <t>Tour0027</t>
+  </si>
+  <si>
+    <t>Tour0026</t>
+  </si>
+  <si>
+    <t>Tour0025</t>
+  </si>
+  <si>
+    <t>Tour0024</t>
+  </si>
+  <si>
+    <t>Tour0023</t>
+  </si>
+  <si>
+    <t>Tour0022</t>
+  </si>
+  <si>
+    <t>As a user, I should be able to request to join a tour</t>
+  </si>
+  <si>
+    <t>As a user, I should be able to add tours and upload photos to the tour</t>
+  </si>
+  <si>
+    <t>As a user I should be able to see a tour's complete details with photos</t>
+  </si>
+  <si>
+    <t>Remove 'See Photos' button link from tour list item beside View Details</t>
+  </si>
+  <si>
+    <t>As a tour creator, I should be able to add schedules to my tour</t>
+  </si>
+  <si>
+    <t>Implement logging functionality</t>
+  </si>
+  <si>
+    <t>Require at least one photo when adding a new tour</t>
+  </si>
+  <si>
+    <t>As a tour creator, I should be able to Add/Remove tour photos after creation</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Tour</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Edit Details</t>
+  </si>
+  <si>
+    <t>Add Details</t>
+  </si>
+  <si>
+    <t>Photos</t>
   </si>
 </sst>
 </file>
@@ -1090,13 +1206,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L290"/>
+  <dimension ref="A1:L307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1169,17 +1285,11 @@
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
@@ -1187,20 +1297,20 @@
       <c r="K3" s="2"/>
       <c r="L3" s="25"/>
     </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1215,16 +1325,16 @@
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1235,20 +1345,20 @@
       <c r="K5" s="2"/>
       <c r="L5" s="25"/>
     </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -1259,20 +1369,20 @@
       <c r="K6" s="2"/>
       <c r="L6" s="25"/>
     </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -1283,20 +1393,20 @@
       <c r="K7" s="2"/>
       <c r="L7" s="25"/>
     </row>
-    <row r="8" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -1307,20 +1417,22 @@
       <c r="K8" s="2"/>
       <c r="L8" s="25"/>
     </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -1335,16 +1447,16 @@
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -1355,20 +1467,20 @@
       <c r="K10" s="2"/>
       <c r="L10" s="25"/>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -1379,14 +1491,14 @@
       <c r="K11" s="2"/>
       <c r="L11" s="25"/>
     </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>
@@ -1394,31 +1506,27 @@
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="25"/>
     </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1432,11 +1540,21 @@
     <row r="14" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1444,139 +1562,245 @@
       <c r="L14" s="25"/>
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="25"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="26"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="26"/>
+    <row r="16" spans="1:12" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="25"/>
     </row>
-    <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
+      <c r="C19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="25"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="26"/>
-    </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+    <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="25"/>
+    </row>
+    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="25"/>
     </row>
-    <row r="22" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="25"/>
     </row>
-    <row r="23" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
+      <c r="C23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="25"/>
     </row>
-    <row r="24" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="3"/>
+      <c r="C24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1586,11 +1810,21 @@
     <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
       <c r="H25" s="3"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1600,11 +1834,21 @@
     <row r="26" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
+      <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1614,11 +1858,21 @@
     <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1628,11 +1882,21 @@
     <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
+      <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1642,11 +1906,21 @@
     <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
+      <c r="C29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1654,13 +1928,25 @@
       <c r="L29" s="25"/>
     </row>
     <row r="30" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
+      <c r="C30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1695,33 +1981,33 @@
       <c r="K32" s="2"/>
       <c r="L32" s="25"/>
     </row>
-    <row r="33" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="25"/>
-    </row>
-    <row r="34" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="25"/>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="26"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="26"/>
     </row>
     <row r="35" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
@@ -1742,6 +2028,8 @@
       <c r="B36" s="4"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="2"/>
@@ -1763,7 +2051,7 @@
       <c r="K37" s="10"/>
       <c r="L37" s="26"/>
     </row>
-    <row r="38" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="2"/>
@@ -1978,8 +2266,6 @@
       <c r="B53" s="4"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="2"/>
@@ -1987,19 +2273,19 @@
       <c r="K53" s="2"/>
       <c r="L53" s="25"/>
     </row>
-    <row r="54" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="25"/>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="26"/>
     </row>
     <row r="55" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
@@ -2323,19 +2609,19 @@
       <c r="K77" s="2"/>
       <c r="L77" s="25"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="7"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="26"/>
+    <row r="78" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="25"/>
     </row>
     <row r="79" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
@@ -2561,19 +2847,19 @@
       <c r="K94" s="2"/>
       <c r="L94" s="25"/>
     </row>
-    <row r="95" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-      <c r="L95" s="25"/>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="7"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="26"/>
     </row>
     <row r="96" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
@@ -2716,7 +3002,7 @@
       <c r="L105" s="25"/>
     </row>
     <row r="106" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="32"/>
+      <c r="A106" s="2"/>
       <c r="B106" s="4"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -2954,7 +3240,7 @@
       <c r="L122" s="25"/>
     </row>
     <row r="123" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="2"/>
+      <c r="A123" s="32"/>
       <c r="B123" s="4"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -2976,7 +3262,7 @@
       <c r="F124" s="2"/>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
-      <c r="I124" s="6"/>
+      <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
       <c r="L124" s="25"/>
@@ -3003,8 +3289,8 @@
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="3"/>
-      <c r="H126" s="31"/>
-      <c r="I126" s="6"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
       <c r="L126" s="25"/>
@@ -3088,7 +3374,7 @@
       <c r="F132" s="2"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
-      <c r="I132" s="6"/>
+      <c r="I132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
       <c r="L132" s="25"/>
@@ -3214,7 +3500,7 @@
       <c r="F141" s="2"/>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
-      <c r="I141" s="2"/>
+      <c r="I141" s="6"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
       <c r="L141" s="25"/>
@@ -3241,8 +3527,8 @@
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="3"/>
-      <c r="H143" s="3"/>
-      <c r="I143" s="2"/>
+      <c r="H143" s="31"/>
+      <c r="I143" s="6"/>
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
       <c r="L143" s="25"/>
@@ -3270,7 +3556,7 @@
       <c r="F145" s="2"/>
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
-      <c r="I145" s="6"/>
+      <c r="I145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
       <c r="L145" s="25"/>
@@ -3284,7 +3570,7 @@
       <c r="F146" s="2"/>
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
-      <c r="I146" s="6"/>
+      <c r="I146" s="2"/>
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
       <c r="L146" s="25"/>
@@ -3326,7 +3612,7 @@
       <c r="F149" s="2"/>
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
-      <c r="I149" s="2"/>
+      <c r="I149" s="6"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
       <c r="L149" s="25"/>
@@ -3438,7 +3724,7 @@
       <c r="F157" s="2"/>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
-      <c r="I157" s="6"/>
+      <c r="I157" s="2"/>
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
       <c r="L157" s="25"/>
@@ -3446,7 +3732,7 @@
     <row r="158" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="4"/>
-      <c r="C158" s="28"/>
+      <c r="C158" s="2"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -3508,7 +3794,7 @@
       <c r="F162" s="2"/>
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
-      <c r="I162" s="2"/>
+      <c r="I162" s="6"/>
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
       <c r="L162" s="25"/>
@@ -3522,7 +3808,7 @@
       <c r="F163" s="2"/>
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
-      <c r="I163" s="2"/>
+      <c r="I163" s="6"/>
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
       <c r="L163" s="25"/>
@@ -3606,7 +3892,7 @@
       <c r="F169" s="2"/>
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
-      <c r="I169" s="6"/>
+      <c r="I169" s="2"/>
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
       <c r="L169" s="25"/>
@@ -3634,7 +3920,7 @@
       <c r="F171" s="2"/>
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
-      <c r="I171" s="6"/>
+      <c r="I171" s="2"/>
       <c r="J171" s="2"/>
       <c r="K171" s="2"/>
       <c r="L171" s="25"/>
@@ -3676,7 +3962,7 @@
       <c r="F174" s="2"/>
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
-      <c r="I174" s="2"/>
+      <c r="I174" s="6"/>
       <c r="J174" s="2"/>
       <c r="K174" s="2"/>
       <c r="L174" s="25"/>
@@ -3684,7 +3970,7 @@
     <row r="175" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="4"/>
-      <c r="C175" s="2"/>
+      <c r="C175" s="28"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
@@ -3746,7 +4032,7 @@
       <c r="F179" s="2"/>
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
-      <c r="I179" s="6"/>
+      <c r="I179" s="2"/>
       <c r="J179" s="2"/>
       <c r="K179" s="2"/>
       <c r="L179" s="25"/>
@@ -3844,7 +4130,7 @@
       <c r="F186" s="2"/>
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
-      <c r="I186" s="2"/>
+      <c r="I186" s="6"/>
       <c r="J186" s="2"/>
       <c r="K186" s="2"/>
       <c r="L186" s="25"/>
@@ -3872,7 +4158,7 @@
       <c r="F188" s="2"/>
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
-      <c r="I188" s="2"/>
+      <c r="I188" s="6"/>
       <c r="J188" s="2"/>
       <c r="K188" s="2"/>
       <c r="L188" s="25"/>
@@ -3984,7 +4270,7 @@
       <c r="F196" s="2"/>
       <c r="G196" s="3"/>
       <c r="H196" s="3"/>
-      <c r="I196" s="2"/>
+      <c r="I196" s="6"/>
       <c r="J196" s="2"/>
       <c r="K196" s="2"/>
       <c r="L196" s="25"/>
@@ -4390,7 +4676,7 @@
       <c r="F225" s="2"/>
       <c r="G225" s="3"/>
       <c r="H225" s="3"/>
-      <c r="I225" s="6"/>
+      <c r="I225" s="2"/>
       <c r="J225" s="2"/>
       <c r="K225" s="2"/>
       <c r="L225" s="25"/>
@@ -4399,6 +4685,7 @@
       <c r="A226" s="2"/>
       <c r="B226" s="4"/>
       <c r="C226" s="2"/>
+      <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="3"/>
@@ -4408,243 +4695,242 @@
       <c r="K226" s="2"/>
       <c r="L226" s="25"/>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A227" s="7"/>
-      <c r="B227" s="9"/>
-      <c r="C227" s="7"/>
-      <c r="D227" s="7"/>
-      <c r="E227" s="7"/>
-      <c r="F227" s="7"/>
-      <c r="G227" s="8"/>
-      <c r="H227" s="8"/>
-      <c r="I227" s="7"/>
-      <c r="J227" s="7"/>
-      <c r="K227" s="7"/>
-      <c r="L227" s="26"/>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A228" s="7"/>
-      <c r="B228" s="9"/>
-      <c r="C228" s="7"/>
-      <c r="D228" s="7"/>
-      <c r="E228" s="7"/>
-      <c r="F228" s="7"/>
-      <c r="G228" s="8"/>
-      <c r="H228" s="8"/>
-      <c r="I228" s="7"/>
-      <c r="J228" s="7"/>
-      <c r="K228" s="7"/>
-      <c r="L228" s="26"/>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A229" s="10"/>
-      <c r="B229" s="12"/>
-      <c r="C229" s="7"/>
-      <c r="D229" s="7"/>
-      <c r="E229" s="10"/>
-      <c r="F229" s="10"/>
-      <c r="G229" s="11"/>
-      <c r="H229" s="11"/>
-      <c r="I229" s="10"/>
-      <c r="J229" s="10"/>
-      <c r="K229" s="10"/>
-      <c r="L229" s="26"/>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A230" s="7"/>
-      <c r="B230" s="9"/>
-      <c r="C230" s="7"/>
-      <c r="D230" s="7"/>
-      <c r="E230" s="7"/>
-      <c r="F230" s="7"/>
-      <c r="G230" s="8"/>
-      <c r="H230" s="8"/>
-      <c r="I230" s="7"/>
-      <c r="J230" s="7"/>
-      <c r="K230" s="7"/>
-      <c r="L230" s="26"/>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A231" s="7"/>
-      <c r="B231" s="9"/>
-      <c r="C231" s="7"/>
-      <c r="D231" s="7"/>
-      <c r="E231" s="7"/>
-      <c r="F231" s="7"/>
-      <c r="G231" s="8"/>
-      <c r="H231" s="8"/>
-      <c r="I231" s="7"/>
-      <c r="J231" s="7"/>
-      <c r="K231" s="7"/>
-      <c r="L231" s="26"/>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A232" s="7"/>
-      <c r="B232" s="9"/>
-      <c r="C232" s="7"/>
-      <c r="D232" s="7"/>
-      <c r="E232" s="7"/>
-      <c r="F232" s="7"/>
-      <c r="G232" s="8"/>
-      <c r="H232" s="8"/>
-      <c r="I232" s="7"/>
-      <c r="J232" s="7"/>
-      <c r="K232" s="7"/>
-      <c r="L232" s="26"/>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A233" s="7"/>
-      <c r="B233" s="9"/>
-      <c r="C233" s="7"/>
-      <c r="D233" s="7"/>
-      <c r="E233" s="7"/>
-      <c r="F233" s="7"/>
-      <c r="G233" s="8"/>
-      <c r="H233" s="8"/>
-      <c r="I233" s="7"/>
-      <c r="J233" s="7"/>
-      <c r="K233" s="7"/>
-      <c r="L233" s="26"/>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A234" s="7"/>
-      <c r="B234" s="9"/>
-      <c r="C234" s="7"/>
-      <c r="D234" s="7"/>
-      <c r="E234" s="7"/>
-      <c r="F234" s="7"/>
-      <c r="G234" s="8"/>
-      <c r="H234" s="8"/>
-      <c r="I234" s="7"/>
-      <c r="J234" s="7"/>
-      <c r="K234" s="7"/>
-      <c r="L234" s="26"/>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A235" s="7"/>
-      <c r="B235" s="9"/>
-      <c r="C235" s="7"/>
-      <c r="D235" s="7"/>
-      <c r="E235" s="7"/>
-      <c r="F235" s="7"/>
-      <c r="G235" s="8"/>
-      <c r="H235" s="8"/>
-      <c r="I235" s="7"/>
-      <c r="J235" s="7"/>
-      <c r="K235" s="7"/>
-      <c r="L235" s="26"/>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A236" s="7"/>
-      <c r="B236" s="9"/>
-      <c r="C236" s="7"/>
-      <c r="D236" s="7"/>
-      <c r="E236" s="7"/>
-      <c r="F236" s="7"/>
-      <c r="G236" s="8"/>
-      <c r="H236" s="8"/>
-      <c r="I236" s="7"/>
-      <c r="J236" s="7"/>
-      <c r="K236" s="7"/>
-      <c r="L236" s="26"/>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A237" s="7"/>
-      <c r="B237" s="9"/>
-      <c r="C237" s="7"/>
-      <c r="D237" s="7"/>
-      <c r="E237" s="7"/>
-      <c r="F237" s="7"/>
-      <c r="G237" s="8"/>
-      <c r="H237" s="8"/>
-      <c r="I237" s="7"/>
-      <c r="J237" s="7"/>
-      <c r="K237" s="7"/>
-      <c r="L237" s="26"/>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A238" s="7"/>
-      <c r="B238" s="9"/>
-      <c r="C238" s="7"/>
-      <c r="D238" s="7"/>
-      <c r="E238" s="7"/>
-      <c r="F238" s="7"/>
-      <c r="G238" s="8"/>
-      <c r="H238" s="8"/>
-      <c r="I238" s="7"/>
-      <c r="J238" s="7"/>
-      <c r="K238" s="7"/>
-      <c r="L238" s="26"/>
-    </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A239" s="7"/>
-      <c r="B239" s="9"/>
-      <c r="C239" s="7"/>
-      <c r="D239" s="7"/>
-      <c r="E239" s="7"/>
-      <c r="F239" s="7"/>
-      <c r="G239" s="8"/>
-      <c r="H239" s="8"/>
-      <c r="I239" s="7"/>
-      <c r="J239" s="7"/>
-      <c r="K239" s="7"/>
-      <c r="L239" s="26"/>
-    </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A240" s="7"/>
-      <c r="B240" s="9"/>
-      <c r="C240" s="7"/>
-      <c r="D240" s="7"/>
-      <c r="E240" s="7"/>
-      <c r="F240" s="7"/>
-      <c r="G240" s="8"/>
-      <c r="H240" s="8"/>
-      <c r="I240" s="7"/>
-      <c r="J240" s="7"/>
-      <c r="K240" s="7"/>
-      <c r="L240" s="26"/>
-    </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A241" s="7"/>
-      <c r="B241" s="9"/>
-      <c r="C241" s="7"/>
-      <c r="D241" s="7"/>
-      <c r="E241" s="7"/>
-      <c r="F241" s="7"/>
-      <c r="G241" s="8"/>
-      <c r="H241" s="8"/>
-      <c r="I241" s="7"/>
-      <c r="J241" s="7"/>
-      <c r="K241" s="7"/>
-      <c r="L241" s="26"/>
-    </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A242" s="7"/>
-      <c r="B242" s="9"/>
-      <c r="C242" s="7"/>
-      <c r="D242" s="7"/>
-      <c r="E242" s="7"/>
-      <c r="F242" s="7"/>
-      <c r="G242" s="8"/>
-      <c r="H242" s="8"/>
-      <c r="I242" s="7"/>
-      <c r="J242" s="7"/>
-      <c r="K242" s="7"/>
-      <c r="L242" s="26"/>
-    </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A243" s="7"/>
-      <c r="B243" s="9"/>
-      <c r="C243" s="7"/>
-      <c r="D243" s="7"/>
-      <c r="E243" s="7"/>
-      <c r="F243" s="7"/>
-      <c r="G243" s="8"/>
-      <c r="H243" s="8"/>
-      <c r="I243" s="7"/>
-      <c r="J243" s="7"/>
-      <c r="K243" s="7"/>
-      <c r="L243" s="26"/>
+    <row r="227" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="2"/>
+      <c r="B227" s="4"/>
+      <c r="C227" s="2"/>
+      <c r="D227" s="2"/>
+      <c r="E227" s="2"/>
+      <c r="F227" s="2"/>
+      <c r="G227" s="3"/>
+      <c r="H227" s="3"/>
+      <c r="I227" s="2"/>
+      <c r="J227" s="2"/>
+      <c r="K227" s="2"/>
+      <c r="L227" s="25"/>
+    </row>
+    <row r="228" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="2"/>
+      <c r="B228" s="4"/>
+      <c r="C228" s="2"/>
+      <c r="D228" s="2"/>
+      <c r="E228" s="2"/>
+      <c r="F228" s="2"/>
+      <c r="G228" s="3"/>
+      <c r="H228" s="3"/>
+      <c r="I228" s="2"/>
+      <c r="J228" s="2"/>
+      <c r="K228" s="2"/>
+      <c r="L228" s="25"/>
+    </row>
+    <row r="229" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="2"/>
+      <c r="B229" s="4"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="3"/>
+      <c r="H229" s="3"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="25"/>
+    </row>
+    <row r="230" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="2"/>
+      <c r="B230" s="4"/>
+      <c r="C230" s="2"/>
+      <c r="D230" s="2"/>
+      <c r="E230" s="2"/>
+      <c r="F230" s="2"/>
+      <c r="G230" s="3"/>
+      <c r="H230" s="3"/>
+      <c r="I230" s="2"/>
+      <c r="J230" s="2"/>
+      <c r="K230" s="2"/>
+      <c r="L230" s="25"/>
+    </row>
+    <row r="231" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="2"/>
+      <c r="B231" s="4"/>
+      <c r="C231" s="2"/>
+      <c r="D231" s="2"/>
+      <c r="E231" s="2"/>
+      <c r="F231" s="2"/>
+      <c r="G231" s="3"/>
+      <c r="H231" s="3"/>
+      <c r="I231" s="2"/>
+      <c r="J231" s="2"/>
+      <c r="K231" s="2"/>
+      <c r="L231" s="25"/>
+    </row>
+    <row r="232" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="2"/>
+      <c r="B232" s="4"/>
+      <c r="C232" s="2"/>
+      <c r="D232" s="2"/>
+      <c r="E232" s="2"/>
+      <c r="F232" s="2"/>
+      <c r="G232" s="3"/>
+      <c r="H232" s="3"/>
+      <c r="I232" s="2"/>
+      <c r="J232" s="2"/>
+      <c r="K232" s="2"/>
+      <c r="L232" s="25"/>
+    </row>
+    <row r="233" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="2"/>
+      <c r="B233" s="4"/>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
+      <c r="E233" s="2"/>
+      <c r="F233" s="2"/>
+      <c r="G233" s="3"/>
+      <c r="H233" s="3"/>
+      <c r="I233" s="2"/>
+      <c r="J233" s="2"/>
+      <c r="K233" s="2"/>
+      <c r="L233" s="25"/>
+    </row>
+    <row r="234" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="2"/>
+      <c r="B234" s="4"/>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
+      <c r="E234" s="2"/>
+      <c r="F234" s="2"/>
+      <c r="G234" s="3"/>
+      <c r="H234" s="3"/>
+      <c r="I234" s="2"/>
+      <c r="J234" s="2"/>
+      <c r="K234" s="2"/>
+      <c r="L234" s="25"/>
+    </row>
+    <row r="235" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="2"/>
+      <c r="B235" s="4"/>
+      <c r="C235" s="2"/>
+      <c r="D235" s="2"/>
+      <c r="E235" s="2"/>
+      <c r="F235" s="2"/>
+      <c r="G235" s="3"/>
+      <c r="H235" s="3"/>
+      <c r="I235" s="2"/>
+      <c r="J235" s="2"/>
+      <c r="K235" s="2"/>
+      <c r="L235" s="25"/>
+    </row>
+    <row r="236" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="2"/>
+      <c r="B236" s="4"/>
+      <c r="C236" s="2"/>
+      <c r="D236" s="2"/>
+      <c r="E236" s="2"/>
+      <c r="F236" s="2"/>
+      <c r="G236" s="3"/>
+      <c r="H236" s="3"/>
+      <c r="I236" s="2"/>
+      <c r="J236" s="2"/>
+      <c r="K236" s="2"/>
+      <c r="L236" s="25"/>
+    </row>
+    <row r="237" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="2"/>
+      <c r="B237" s="4"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+      <c r="E237" s="2"/>
+      <c r="F237" s="2"/>
+      <c r="G237" s="3"/>
+      <c r="H237" s="3"/>
+      <c r="I237" s="2"/>
+      <c r="J237" s="2"/>
+      <c r="K237" s="2"/>
+      <c r="L237" s="25"/>
+    </row>
+    <row r="238" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="2"/>
+      <c r="B238" s="4"/>
+      <c r="C238" s="2"/>
+      <c r="D238" s="2"/>
+      <c r="E238" s="2"/>
+      <c r="F238" s="2"/>
+      <c r="G238" s="3"/>
+      <c r="H238" s="3"/>
+      <c r="I238" s="2"/>
+      <c r="J238" s="2"/>
+      <c r="K238" s="2"/>
+      <c r="L238" s="25"/>
+    </row>
+    <row r="239" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="2"/>
+      <c r="B239" s="4"/>
+      <c r="C239" s="2"/>
+      <c r="D239" s="2"/>
+      <c r="E239" s="2"/>
+      <c r="F239" s="2"/>
+      <c r="G239" s="3"/>
+      <c r="H239" s="3"/>
+      <c r="I239" s="2"/>
+      <c r="J239" s="2"/>
+      <c r="K239" s="2"/>
+      <c r="L239" s="25"/>
+    </row>
+    <row r="240" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="2"/>
+      <c r="B240" s="4"/>
+      <c r="C240" s="2"/>
+      <c r="D240" s="2"/>
+      <c r="E240" s="2"/>
+      <c r="F240" s="2"/>
+      <c r="G240" s="3"/>
+      <c r="H240" s="3"/>
+      <c r="I240" s="2"/>
+      <c r="J240" s="2"/>
+      <c r="K240" s="2"/>
+      <c r="L240" s="25"/>
+    </row>
+    <row r="241" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="2"/>
+      <c r="B241" s="4"/>
+      <c r="C241" s="2"/>
+      <c r="D241" s="2"/>
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="3"/>
+      <c r="H241" s="3"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="25"/>
+    </row>
+    <row r="242" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="2"/>
+      <c r="B242" s="4"/>
+      <c r="C242" s="2"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="2"/>
+      <c r="F242" s="2"/>
+      <c r="G242" s="3"/>
+      <c r="H242" s="3"/>
+      <c r="I242" s="6"/>
+      <c r="J242" s="2"/>
+      <c r="K242" s="2"/>
+      <c r="L242" s="25"/>
+    </row>
+    <row r="243" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="2"/>
+      <c r="B243" s="4"/>
+      <c r="C243" s="2"/>
+      <c r="E243" s="2"/>
+      <c r="F243" s="2"/>
+      <c r="G243" s="3"/>
+      <c r="H243" s="3"/>
+      <c r="I243" s="2"/>
+      <c r="J243" s="2"/>
+      <c r="K243" s="2"/>
+      <c r="L243" s="25"/>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" s="7"/>
@@ -4675,17 +4961,17 @@
       <c r="L245" s="26"/>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A246" s="7"/>
-      <c r="B246" s="9"/>
+      <c r="A246" s="10"/>
+      <c r="B246" s="12"/>
       <c r="C246" s="7"/>
       <c r="D246" s="7"/>
-      <c r="E246" s="7"/>
-      <c r="F246" s="7"/>
-      <c r="G246" s="8"/>
-      <c r="H246" s="8"/>
-      <c r="I246" s="7"/>
-      <c r="J246" s="7"/>
-      <c r="K246" s="7"/>
+      <c r="E246" s="10"/>
+      <c r="F246" s="10"/>
+      <c r="G246" s="11"/>
+      <c r="H246" s="11"/>
+      <c r="I246" s="10"/>
+      <c r="J246" s="10"/>
+      <c r="K246" s="10"/>
       <c r="L246" s="26"/>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.3">
@@ -4723,8 +5009,8 @@
       <c r="D249" s="7"/>
       <c r="E249" s="7"/>
       <c r="F249" s="7"/>
-      <c r="G249" s="11"/>
-      <c r="H249" s="11"/>
+      <c r="G249" s="8"/>
+      <c r="H249" s="8"/>
       <c r="I249" s="7"/>
       <c r="J249" s="7"/>
       <c r="K249" s="7"/>
@@ -4747,141 +5033,141 @@
     <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" s="7"/>
       <c r="B251" s="9"/>
-      <c r="C251" s="10"/>
-      <c r="D251" s="10"/>
-      <c r="E251" s="10"/>
-      <c r="F251" s="10"/>
-      <c r="G251" s="11"/>
-      <c r="H251" s="11"/>
-      <c r="I251" s="10"/>
-      <c r="J251" s="10"/>
-      <c r="K251" s="10"/>
+      <c r="C251" s="7"/>
+      <c r="D251" s="7"/>
+      <c r="E251" s="7"/>
+      <c r="F251" s="7"/>
+      <c r="G251" s="8"/>
+      <c r="H251" s="8"/>
+      <c r="I251" s="7"/>
+      <c r="J251" s="7"/>
+      <c r="K251" s="7"/>
       <c r="L251" s="26"/>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" s="7"/>
       <c r="B252" s="9"/>
-      <c r="C252" s="10"/>
-      <c r="D252" s="10"/>
-      <c r="E252" s="10"/>
-      <c r="F252" s="10"/>
-      <c r="G252" s="11"/>
-      <c r="H252" s="11"/>
-      <c r="I252" s="10"/>
-      <c r="J252" s="10"/>
-      <c r="K252" s="10"/>
+      <c r="C252" s="7"/>
+      <c r="D252" s="7"/>
+      <c r="E252" s="7"/>
+      <c r="F252" s="7"/>
+      <c r="G252" s="8"/>
+      <c r="H252" s="8"/>
+      <c r="I252" s="7"/>
+      <c r="J252" s="7"/>
+      <c r="K252" s="7"/>
       <c r="L252" s="26"/>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" s="7"/>
-      <c r="B253" s="12"/>
-      <c r="C253" s="10"/>
-      <c r="D253" s="10"/>
-      <c r="E253" s="10"/>
-      <c r="F253" s="10"/>
-      <c r="G253" s="11"/>
-      <c r="H253" s="11"/>
-      <c r="I253" s="10"/>
-      <c r="J253" s="10"/>
-      <c r="K253" s="10"/>
+      <c r="B253" s="9"/>
+      <c r="C253" s="7"/>
+      <c r="D253" s="7"/>
+      <c r="E253" s="7"/>
+      <c r="F253" s="7"/>
+      <c r="G253" s="8"/>
+      <c r="H253" s="8"/>
+      <c r="I253" s="7"/>
+      <c r="J253" s="7"/>
+      <c r="K253" s="7"/>
       <c r="L253" s="26"/>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" s="7"/>
-      <c r="B254" s="12"/>
-      <c r="C254" s="10"/>
-      <c r="D254" s="10"/>
-      <c r="E254" s="10"/>
-      <c r="F254" s="10"/>
-      <c r="G254" s="11"/>
-      <c r="H254" s="11"/>
-      <c r="I254" s="10"/>
-      <c r="J254" s="10"/>
-      <c r="K254" s="10"/>
+      <c r="B254" s="9"/>
+      <c r="C254" s="7"/>
+      <c r="D254" s="7"/>
+      <c r="E254" s="7"/>
+      <c r="F254" s="7"/>
+      <c r="G254" s="8"/>
+      <c r="H254" s="8"/>
+      <c r="I254" s="7"/>
+      <c r="J254" s="7"/>
+      <c r="K254" s="7"/>
       <c r="L254" s="26"/>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" s="7"/>
-      <c r="B255" s="12"/>
-      <c r="C255" s="10"/>
-      <c r="D255" s="10"/>
-      <c r="E255" s="10"/>
-      <c r="F255" s="10"/>
-      <c r="G255" s="11"/>
-      <c r="H255" s="11"/>
-      <c r="I255" s="10"/>
-      <c r="J255" s="10"/>
-      <c r="K255" s="10"/>
+      <c r="B255" s="9"/>
+      <c r="C255" s="7"/>
+      <c r="D255" s="7"/>
+      <c r="E255" s="7"/>
+      <c r="F255" s="7"/>
+      <c r="G255" s="8"/>
+      <c r="H255" s="8"/>
+      <c r="I255" s="7"/>
+      <c r="J255" s="7"/>
+      <c r="K255" s="7"/>
       <c r="L255" s="26"/>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" s="7"/>
-      <c r="B256" s="12"/>
-      <c r="C256" s="10"/>
-      <c r="D256" s="10"/>
-      <c r="E256" s="10"/>
-      <c r="F256" s="10"/>
-      <c r="G256" s="11"/>
-      <c r="H256" s="11"/>
-      <c r="I256" s="13"/>
-      <c r="J256" s="10"/>
-      <c r="K256" s="10"/>
+      <c r="B256" s="9"/>
+      <c r="C256" s="7"/>
+      <c r="D256" s="7"/>
+      <c r="E256" s="7"/>
+      <c r="F256" s="7"/>
+      <c r="G256" s="8"/>
+      <c r="H256" s="8"/>
+      <c r="I256" s="7"/>
+      <c r="J256" s="7"/>
+      <c r="K256" s="7"/>
       <c r="L256" s="26"/>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" s="7"/>
-      <c r="B257" s="12"/>
-      <c r="C257" s="10"/>
-      <c r="D257" s="10"/>
-      <c r="E257" s="10"/>
-      <c r="F257" s="10"/>
-      <c r="G257" s="11"/>
-      <c r="H257" s="11"/>
-      <c r="I257" s="10"/>
-      <c r="J257" s="10"/>
-      <c r="K257" s="10"/>
+      <c r="B257" s="9"/>
+      <c r="C257" s="7"/>
+      <c r="D257" s="7"/>
+      <c r="E257" s="7"/>
+      <c r="F257" s="7"/>
+      <c r="G257" s="8"/>
+      <c r="H257" s="8"/>
+      <c r="I257" s="7"/>
+      <c r="J257" s="7"/>
+      <c r="K257" s="7"/>
       <c r="L257" s="26"/>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" s="7"/>
-      <c r="B258" s="12"/>
-      <c r="C258" s="10"/>
-      <c r="D258" s="10"/>
-      <c r="E258" s="10"/>
-      <c r="F258" s="10"/>
-      <c r="G258" s="11"/>
-      <c r="H258" s="11"/>
-      <c r="I258" s="14"/>
-      <c r="J258" s="10"/>
-      <c r="K258" s="10"/>
+      <c r="B258" s="9"/>
+      <c r="C258" s="7"/>
+      <c r="D258" s="7"/>
+      <c r="E258" s="7"/>
+      <c r="F258" s="7"/>
+      <c r="G258" s="8"/>
+      <c r="H258" s="8"/>
+      <c r="I258" s="7"/>
+      <c r="J258" s="7"/>
+      <c r="K258" s="7"/>
       <c r="L258" s="26"/>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" s="7"/>
-      <c r="B259" s="12"/>
-      <c r="C259" s="10"/>
-      <c r="D259" s="10"/>
-      <c r="E259" s="10"/>
-      <c r="F259" s="10"/>
-      <c r="G259" s="11"/>
-      <c r="H259" s="11"/>
-      <c r="I259" s="13"/>
-      <c r="J259" s="10"/>
-      <c r="K259" s="10"/>
+      <c r="B259" s="9"/>
+      <c r="C259" s="7"/>
+      <c r="D259" s="7"/>
+      <c r="E259" s="7"/>
+      <c r="F259" s="7"/>
+      <c r="G259" s="8"/>
+      <c r="H259" s="8"/>
+      <c r="I259" s="7"/>
+      <c r="J259" s="7"/>
+      <c r="K259" s="7"/>
       <c r="L259" s="26"/>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" s="7"/>
-      <c r="B260" s="12"/>
-      <c r="C260" s="10"/>
-      <c r="D260" s="10"/>
-      <c r="E260" s="10"/>
-      <c r="F260" s="10"/>
-      <c r="G260" s="11"/>
-      <c r="H260" s="11"/>
-      <c r="I260" s="10"/>
-      <c r="J260" s="10"/>
-      <c r="K260" s="10"/>
+      <c r="B260" s="9"/>
+      <c r="C260" s="7"/>
+      <c r="D260" s="7"/>
+      <c r="E260" s="7"/>
+      <c r="F260" s="7"/>
+      <c r="G260" s="8"/>
+      <c r="H260" s="8"/>
+      <c r="I260" s="7"/>
+      <c r="J260" s="7"/>
+      <c r="K260" s="7"/>
       <c r="L260" s="26"/>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.3">
@@ -4900,91 +5186,91 @@
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" s="7"/>
-      <c r="B262" s="12"/>
-      <c r="C262" s="10"/>
-      <c r="D262" s="10"/>
-      <c r="E262" s="10"/>
-      <c r="F262" s="10"/>
-      <c r="G262" s="11"/>
-      <c r="H262" s="11"/>
-      <c r="I262" s="10"/>
-      <c r="J262" s="10"/>
-      <c r="K262" s="10"/>
+      <c r="B262" s="9"/>
+      <c r="C262" s="7"/>
+      <c r="D262" s="7"/>
+      <c r="E262" s="7"/>
+      <c r="F262" s="7"/>
+      <c r="G262" s="8"/>
+      <c r="H262" s="8"/>
+      <c r="I262" s="7"/>
+      <c r="J262" s="7"/>
+      <c r="K262" s="7"/>
       <c r="L262" s="26"/>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" s="7"/>
-      <c r="B263" s="12"/>
-      <c r="C263" s="10"/>
-      <c r="D263" s="10"/>
-      <c r="E263" s="10"/>
-      <c r="F263" s="10"/>
-      <c r="G263" s="11"/>
-      <c r="H263" s="11"/>
-      <c r="I263" s="10"/>
-      <c r="J263" s="10"/>
-      <c r="K263" s="10"/>
+      <c r="B263" s="9"/>
+      <c r="C263" s="7"/>
+      <c r="D263" s="7"/>
+      <c r="E263" s="7"/>
+      <c r="F263" s="7"/>
+      <c r="G263" s="8"/>
+      <c r="H263" s="8"/>
+      <c r="I263" s="7"/>
+      <c r="J263" s="7"/>
+      <c r="K263" s="7"/>
       <c r="L263" s="26"/>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" s="7"/>
-      <c r="B264" s="12"/>
-      <c r="C264" s="10"/>
-      <c r="D264" s="10"/>
-      <c r="E264" s="10"/>
-      <c r="F264" s="10"/>
-      <c r="G264" s="11"/>
-      <c r="H264" s="11"/>
-      <c r="I264" s="10"/>
-      <c r="J264" s="10"/>
-      <c r="K264" s="10"/>
+      <c r="B264" s="9"/>
+      <c r="C264" s="7"/>
+      <c r="D264" s="7"/>
+      <c r="E264" s="7"/>
+      <c r="F264" s="7"/>
+      <c r="G264" s="8"/>
+      <c r="H264" s="8"/>
+      <c r="I264" s="7"/>
+      <c r="J264" s="7"/>
+      <c r="K264" s="7"/>
       <c r="L264" s="26"/>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" s="7"/>
-      <c r="B265" s="12"/>
-      <c r="C265" s="10"/>
-      <c r="D265" s="10"/>
-      <c r="E265" s="10"/>
-      <c r="F265" s="10"/>
-      <c r="G265" s="11"/>
-      <c r="H265" s="11"/>
-      <c r="I265" s="10"/>
-      <c r="J265" s="10"/>
-      <c r="K265" s="10"/>
+      <c r="B265" s="9"/>
+      <c r="C265" s="7"/>
+      <c r="D265" s="7"/>
+      <c r="E265" s="7"/>
+      <c r="F265" s="7"/>
+      <c r="G265" s="8"/>
+      <c r="H265" s="8"/>
+      <c r="I265" s="7"/>
+      <c r="J265" s="7"/>
+      <c r="K265" s="7"/>
       <c r="L265" s="26"/>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" s="7"/>
-      <c r="B266" s="12"/>
-      <c r="C266" s="10"/>
-      <c r="D266" s="10"/>
-      <c r="E266" s="10"/>
-      <c r="F266" s="10"/>
+      <c r="B266" s="9"/>
+      <c r="C266" s="7"/>
+      <c r="D266" s="7"/>
+      <c r="E266" s="7"/>
+      <c r="F266" s="7"/>
       <c r="G266" s="11"/>
       <c r="H266" s="11"/>
-      <c r="I266" s="10"/>
-      <c r="J266" s="10"/>
-      <c r="K266" s="10"/>
+      <c r="I266" s="7"/>
+      <c r="J266" s="7"/>
+      <c r="K266" s="7"/>
       <c r="L266" s="26"/>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267" s="7"/>
-      <c r="B267" s="12"/>
-      <c r="C267" s="10"/>
-      <c r="D267" s="10"/>
-      <c r="E267" s="10"/>
-      <c r="F267" s="10"/>
-      <c r="G267" s="11"/>
-      <c r="H267" s="11"/>
-      <c r="I267" s="10"/>
-      <c r="J267" s="10"/>
-      <c r="K267" s="10"/>
+      <c r="B267" s="9"/>
+      <c r="C267" s="7"/>
+      <c r="D267" s="7"/>
+      <c r="E267" s="7"/>
+      <c r="F267" s="7"/>
+      <c r="G267" s="8"/>
+      <c r="H267" s="8"/>
+      <c r="I267" s="7"/>
+      <c r="J267" s="7"/>
+      <c r="K267" s="7"/>
       <c r="L267" s="26"/>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268" s="7"/>
-      <c r="B268" s="12"/>
+      <c r="B268" s="9"/>
       <c r="C268" s="10"/>
       <c r="D268" s="10"/>
       <c r="E268" s="10"/>
@@ -4998,7 +5284,7 @@
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269" s="7"/>
-      <c r="B269" s="12"/>
+      <c r="B269" s="9"/>
       <c r="C269" s="10"/>
       <c r="D269" s="10"/>
       <c r="E269" s="10"/>
@@ -5019,7 +5305,7 @@
       <c r="F270" s="10"/>
       <c r="G270" s="11"/>
       <c r="H270" s="11"/>
-      <c r="I270" s="15"/>
+      <c r="I270" s="10"/>
       <c r="J270" s="10"/>
       <c r="K270" s="10"/>
       <c r="L270" s="26"/>
@@ -5032,8 +5318,8 @@
       <c r="E271" s="10"/>
       <c r="F271" s="10"/>
       <c r="G271" s="11"/>
-      <c r="H271" s="29"/>
-      <c r="I271" s="16"/>
+      <c r="H271" s="11"/>
+      <c r="I271" s="10"/>
       <c r="J271" s="10"/>
       <c r="K271" s="10"/>
       <c r="L271" s="26"/>
@@ -5061,7 +5347,7 @@
       <c r="F273" s="10"/>
       <c r="G273" s="11"/>
       <c r="H273" s="11"/>
-      <c r="I273" s="10"/>
+      <c r="I273" s="13"/>
       <c r="J273" s="10"/>
       <c r="K273" s="10"/>
       <c r="L273" s="26"/>
@@ -5070,7 +5356,7 @@
       <c r="A274" s="7"/>
       <c r="B274" s="12"/>
       <c r="C274" s="10"/>
-      <c r="D274" s="16"/>
+      <c r="D274" s="10"/>
       <c r="E274" s="10"/>
       <c r="F274" s="10"/>
       <c r="G274" s="11"/>
@@ -5082,14 +5368,14 @@
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A275" s="7"/>
-      <c r="B275" s="9"/>
-      <c r="C275" s="7"/>
-      <c r="D275" s="7"/>
-      <c r="E275" s="7"/>
-      <c r="F275" s="7"/>
-      <c r="G275" s="8"/>
-      <c r="H275" s="8"/>
-      <c r="I275" s="10"/>
+      <c r="B275" s="12"/>
+      <c r="C275" s="10"/>
+      <c r="D275" s="10"/>
+      <c r="E275" s="10"/>
+      <c r="F275" s="10"/>
+      <c r="G275" s="11"/>
+      <c r="H275" s="11"/>
+      <c r="I275" s="14"/>
       <c r="J275" s="10"/>
       <c r="K275" s="10"/>
       <c r="L275" s="26"/>
@@ -5103,7 +5389,7 @@
       <c r="F276" s="10"/>
       <c r="G276" s="11"/>
       <c r="H276" s="11"/>
-      <c r="I276" s="10"/>
+      <c r="I276" s="13"/>
       <c r="J276" s="10"/>
       <c r="K276" s="10"/>
       <c r="L276" s="26"/>
@@ -5124,16 +5410,16 @@
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" s="7"/>
-      <c r="B278" s="12"/>
-      <c r="C278" s="10"/>
-      <c r="D278" s="10"/>
-      <c r="E278" s="10"/>
-      <c r="F278" s="10"/>
-      <c r="G278" s="11"/>
-      <c r="H278" s="11"/>
-      <c r="I278" s="10"/>
-      <c r="J278" s="10"/>
-      <c r="K278" s="10"/>
+      <c r="B278" s="9"/>
+      <c r="C278" s="7"/>
+      <c r="D278" s="7"/>
+      <c r="E278" s="7"/>
+      <c r="F278" s="7"/>
+      <c r="G278" s="8"/>
+      <c r="H278" s="8"/>
+      <c r="I278" s="7"/>
+      <c r="J278" s="7"/>
+      <c r="K278" s="7"/>
       <c r="L278" s="26"/>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
@@ -5165,7 +5451,7 @@
       <c r="L280" s="26"/>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A281" s="10"/>
+      <c r="A281" s="7"/>
       <c r="B281" s="12"/>
       <c r="C281" s="10"/>
       <c r="D281" s="10"/>
@@ -5179,7 +5465,7 @@
       <c r="L281" s="26"/>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A282" s="10"/>
+      <c r="A282" s="7"/>
       <c r="B282" s="12"/>
       <c r="C282" s="10"/>
       <c r="D282" s="10"/>
@@ -5193,7 +5479,7 @@
       <c r="L282" s="26"/>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A283" s="10"/>
+      <c r="A283" s="7"/>
       <c r="B283" s="12"/>
       <c r="C283" s="10"/>
       <c r="D283" s="10"/>
@@ -5207,7 +5493,7 @@
       <c r="L283" s="26"/>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A284" s="10"/>
+      <c r="A284" s="7"/>
       <c r="B284" s="12"/>
       <c r="C284" s="10"/>
       <c r="D284" s="10"/>
@@ -5221,7 +5507,7 @@
       <c r="L284" s="26"/>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A285" s="10"/>
+      <c r="A285" s="7"/>
       <c r="B285" s="12"/>
       <c r="C285" s="10"/>
       <c r="D285" s="10"/>
@@ -5235,21 +5521,21 @@
       <c r="L285" s="26"/>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A286" s="10"/>
+      <c r="A286" s="7"/>
       <c r="B286" s="12"/>
       <c r="C286" s="10"/>
       <c r="D286" s="10"/>
       <c r="E286" s="10"/>
       <c r="F286" s="10"/>
       <c r="G286" s="11"/>
-      <c r="H286" s="29"/>
-      <c r="I286" s="16"/>
+      <c r="H286" s="11"/>
+      <c r="I286" s="10"/>
       <c r="J286" s="10"/>
       <c r="K286" s="10"/>
       <c r="L286" s="26"/>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A287" s="10"/>
+      <c r="A287" s="7"/>
       <c r="B287" s="12"/>
       <c r="C287" s="10"/>
       <c r="D287" s="10"/>
@@ -5257,27 +5543,27 @@
       <c r="F287" s="10"/>
       <c r="G287" s="11"/>
       <c r="H287" s="11"/>
-      <c r="I287" s="10"/>
+      <c r="I287" s="15"/>
       <c r="J287" s="10"/>
       <c r="K287" s="10"/>
       <c r="L287" s="26"/>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A288" s="10"/>
+      <c r="A288" s="7"/>
       <c r="B288" s="12"/>
       <c r="C288" s="10"/>
       <c r="D288" s="10"/>
       <c r="E288" s="10"/>
       <c r="F288" s="10"/>
       <c r="G288" s="11"/>
-      <c r="H288" s="11"/>
-      <c r="I288" s="10"/>
+      <c r="H288" s="29"/>
+      <c r="I288" s="16"/>
       <c r="J288" s="10"/>
       <c r="K288" s="10"/>
       <c r="L288" s="26"/>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A289" s="10"/>
+      <c r="A289" s="7"/>
       <c r="B289" s="12"/>
       <c r="C289" s="10"/>
       <c r="D289" s="10"/>
@@ -5291,25 +5577,263 @@
       <c r="L289" s="26"/>
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A290" s="17"/>
-      <c r="B290" s="17"/>
-      <c r="C290" s="17"/>
-      <c r="D290" s="17"/>
-      <c r="E290" s="17"/>
-      <c r="F290" s="17"/>
-      <c r="G290" s="18"/>
-      <c r="H290" s="18"/>
-      <c r="I290" s="17"/>
-      <c r="J290" s="17"/>
-      <c r="K290" s="17"/>
+      <c r="A290" s="7"/>
+      <c r="B290" s="12"/>
+      <c r="C290" s="10"/>
+      <c r="D290" s="10"/>
+      <c r="E290" s="10"/>
+      <c r="F290" s="10"/>
+      <c r="G290" s="11"/>
+      <c r="H290" s="11"/>
+      <c r="I290" s="10"/>
+      <c r="J290" s="10"/>
+      <c r="K290" s="10"/>
+      <c r="L290" s="26"/>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A291" s="7"/>
+      <c r="B291" s="12"/>
+      <c r="C291" s="10"/>
+      <c r="D291" s="16"/>
+      <c r="E291" s="10"/>
+      <c r="F291" s="10"/>
+      <c r="G291" s="11"/>
+      <c r="H291" s="11"/>
+      <c r="I291" s="10"/>
+      <c r="J291" s="10"/>
+      <c r="K291" s="10"/>
+      <c r="L291" s="26"/>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A292" s="7"/>
+      <c r="B292" s="9"/>
+      <c r="C292" s="7"/>
+      <c r="D292" s="7"/>
+      <c r="E292" s="7"/>
+      <c r="F292" s="7"/>
+      <c r="G292" s="8"/>
+      <c r="H292" s="8"/>
+      <c r="I292" s="10"/>
+      <c r="J292" s="10"/>
+      <c r="K292" s="10"/>
+      <c r="L292" s="26"/>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A293" s="7"/>
+      <c r="B293" s="12"/>
+      <c r="C293" s="10"/>
+      <c r="D293" s="10"/>
+      <c r="E293" s="10"/>
+      <c r="F293" s="10"/>
+      <c r="G293" s="11"/>
+      <c r="H293" s="11"/>
+      <c r="I293" s="10"/>
+      <c r="J293" s="10"/>
+      <c r="K293" s="10"/>
+      <c r="L293" s="26"/>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A294" s="7"/>
+      <c r="B294" s="12"/>
+      <c r="C294" s="10"/>
+      <c r="D294" s="10"/>
+      <c r="E294" s="10"/>
+      <c r="F294" s="10"/>
+      <c r="G294" s="11"/>
+      <c r="H294" s="11"/>
+      <c r="I294" s="10"/>
+      <c r="J294" s="10"/>
+      <c r="K294" s="10"/>
+      <c r="L294" s="26"/>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A295" s="7"/>
+      <c r="B295" s="12"/>
+      <c r="C295" s="10"/>
+      <c r="D295" s="10"/>
+      <c r="E295" s="10"/>
+      <c r="F295" s="10"/>
+      <c r="G295" s="11"/>
+      <c r="H295" s="11"/>
+      <c r="I295" s="10"/>
+      <c r="J295" s="10"/>
+      <c r="K295" s="10"/>
+      <c r="L295" s="26"/>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A296" s="7"/>
+      <c r="B296" s="12"/>
+      <c r="C296" s="10"/>
+      <c r="D296" s="10"/>
+      <c r="E296" s="10"/>
+      <c r="F296" s="10"/>
+      <c r="G296" s="11"/>
+      <c r="H296" s="11"/>
+      <c r="I296" s="10"/>
+      <c r="J296" s="10"/>
+      <c r="K296" s="10"/>
+      <c r="L296" s="26"/>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A297" s="7"/>
+      <c r="B297" s="12"/>
+      <c r="C297" s="10"/>
+      <c r="D297" s="10"/>
+      <c r="E297" s="10"/>
+      <c r="F297" s="10"/>
+      <c r="G297" s="11"/>
+      <c r="H297" s="11"/>
+      <c r="I297" s="10"/>
+      <c r="J297" s="10"/>
+      <c r="K297" s="10"/>
+      <c r="L297" s="26"/>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A298" s="10"/>
+      <c r="B298" s="12"/>
+      <c r="C298" s="10"/>
+      <c r="D298" s="10"/>
+      <c r="E298" s="10"/>
+      <c r="F298" s="10"/>
+      <c r="G298" s="11"/>
+      <c r="H298" s="11"/>
+      <c r="I298" s="10"/>
+      <c r="J298" s="10"/>
+      <c r="K298" s="10"/>
+      <c r="L298" s="26"/>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A299" s="10"/>
+      <c r="B299" s="12"/>
+      <c r="C299" s="10"/>
+      <c r="D299" s="10"/>
+      <c r="E299" s="10"/>
+      <c r="F299" s="10"/>
+      <c r="G299" s="11"/>
+      <c r="H299" s="11"/>
+      <c r="I299" s="10"/>
+      <c r="J299" s="10"/>
+      <c r="K299" s="10"/>
+      <c r="L299" s="26"/>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A300" s="10"/>
+      <c r="B300" s="12"/>
+      <c r="C300" s="10"/>
+      <c r="D300" s="10"/>
+      <c r="E300" s="10"/>
+      <c r="F300" s="10"/>
+      <c r="G300" s="11"/>
+      <c r="H300" s="11"/>
+      <c r="I300" s="10"/>
+      <c r="J300" s="10"/>
+      <c r="K300" s="10"/>
+      <c r="L300" s="26"/>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A301" s="10"/>
+      <c r="B301" s="12"/>
+      <c r="C301" s="10"/>
+      <c r="D301" s="10"/>
+      <c r="E301" s="10"/>
+      <c r="F301" s="10"/>
+      <c r="G301" s="11"/>
+      <c r="H301" s="11"/>
+      <c r="I301" s="10"/>
+      <c r="J301" s="10"/>
+      <c r="K301" s="10"/>
+      <c r="L301" s="26"/>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A302" s="10"/>
+      <c r="B302" s="12"/>
+      <c r="C302" s="10"/>
+      <c r="D302" s="10"/>
+      <c r="E302" s="10"/>
+      <c r="F302" s="10"/>
+      <c r="G302" s="11"/>
+      <c r="H302" s="11"/>
+      <c r="I302" s="10"/>
+      <c r="J302" s="10"/>
+      <c r="K302" s="10"/>
+      <c r="L302" s="26"/>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A303" s="10"/>
+      <c r="B303" s="12"/>
+      <c r="C303" s="10"/>
+      <c r="D303" s="10"/>
+      <c r="E303" s="10"/>
+      <c r="F303" s="10"/>
+      <c r="G303" s="11"/>
+      <c r="H303" s="29"/>
+      <c r="I303" s="16"/>
+      <c r="J303" s="10"/>
+      <c r="K303" s="10"/>
+      <c r="L303" s="26"/>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A304" s="10"/>
+      <c r="B304" s="12"/>
+      <c r="C304" s="10"/>
+      <c r="D304" s="10"/>
+      <c r="E304" s="10"/>
+      <c r="F304" s="10"/>
+      <c r="G304" s="11"/>
+      <c r="H304" s="11"/>
+      <c r="I304" s="10"/>
+      <c r="J304" s="10"/>
+      <c r="K304" s="10"/>
+      <c r="L304" s="26"/>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A305" s="10"/>
+      <c r="B305" s="12"/>
+      <c r="C305" s="10"/>
+      <c r="D305" s="10"/>
+      <c r="E305" s="10"/>
+      <c r="F305" s="10"/>
+      <c r="G305" s="11"/>
+      <c r="H305" s="11"/>
+      <c r="I305" s="10"/>
+      <c r="J305" s="10"/>
+      <c r="K305" s="10"/>
+      <c r="L305" s="26"/>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A306" s="10"/>
+      <c r="B306" s="12"/>
+      <c r="C306" s="10"/>
+      <c r="D306" s="10"/>
+      <c r="E306" s="10"/>
+      <c r="F306" s="10"/>
+      <c r="G306" s="11"/>
+      <c r="H306" s="11"/>
+      <c r="I306" s="10"/>
+      <c r="J306" s="10"/>
+      <c r="K306" s="10"/>
+      <c r="L306" s="26"/>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A307" s="17"/>
+      <c r="B307" s="17"/>
+      <c r="C307" s="17"/>
+      <c r="D307" s="17"/>
+      <c r="E307" s="17"/>
+      <c r="F307" s="17"/>
+      <c r="G307" s="18"/>
+      <c r="H307" s="18"/>
+      <c r="I307" s="17"/>
+      <c r="J307" s="17"/>
+      <c r="K307" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L290" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A103:K104">
-    <sortCondition descending="1" ref="C103:C104"/>
+  <autoFilter ref="A1:L307" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A120:K121">
+    <sortCondition descending="1" ref="C120:C121"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="A137:A289 A102:A134 A2:A100">
+  <conditionalFormatting sqref="A154:A306 A119:A151 A2:A117">
     <cfRule type="cellIs" dxfId="30" priority="47" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
@@ -5320,12 +5844,12 @@
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B137:B289 B102:B135 B2:B100">
+  <conditionalFormatting sqref="B154:B306 B119:B152 B2:B117">
     <cfRule type="expression" dxfId="27" priority="48">
       <formula>AND($A2 = "Done", ISBLANK($B2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E102:E289 E2:E100">
+  <conditionalFormatting sqref="E119:E306 E2:E117">
     <cfRule type="expression" dxfId="26" priority="42">
       <formula>$E2="Improv"</formula>
     </cfRule>
@@ -5342,7 +5866,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F102:F289 F2:F100">
+  <conditionalFormatting sqref="F119:F306 F2:F117">
     <cfRule type="cellIs" dxfId="21" priority="35" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -5356,78 +5880,78 @@
       <formula>LEN(TRIM(F2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A135">
+  <conditionalFormatting sqref="A152">
     <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="17" priority="20" stopIfTrue="1">
-      <formula>LEN(TRIM(A135))=0</formula>
+      <formula>LEN(TRIM(A152))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B136">
+  <conditionalFormatting sqref="B153">
     <cfRule type="expression" dxfId="15" priority="17">
-      <formula>AND($A136 = "Done", ISBLANK($B136))</formula>
+      <formula>AND($A153 = "Done", ISBLANK($B153))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A136">
+  <conditionalFormatting sqref="A153">
     <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="13" priority="15" stopIfTrue="1">
-      <formula>LEN(TRIM(A136))=0</formula>
+      <formula>LEN(TRIM(A153))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
+  <conditionalFormatting sqref="A118">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Started"</formula>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="10" priority="12" stopIfTrue="1">
-      <formula>LEN(TRIM(A101))=0</formula>
+      <formula>LEN(TRIM(A118))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B101">
+  <conditionalFormatting sqref="B118">
     <cfRule type="expression" dxfId="8" priority="11">
-      <formula>AND($A101 = "Done", ISBLANK($B101))</formula>
+      <formula>AND($A118 = "Done", ISBLANK($B118))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E101">
+  <conditionalFormatting sqref="E118">
     <cfRule type="expression" dxfId="7" priority="5">
-      <formula>$E101="Improv"</formula>
+      <formula>$E118="Improv"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
-      <formula>$E101="Feat"</formula>
+      <formula>$E118="Feat"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
-      <formula>$E101="Design"</formula>
+      <formula>$E118="Design"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
-      <formula>$E101="Bug"</formula>
+      <formula>$E118="Bug"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="9">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101">
+  <conditionalFormatting sqref="F118">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>$F101="High"</formula>
+      <formula>$F118="High"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>$F101="Medium"</formula>
+      <formula>$F118="Medium"</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="4">
-      <formula>LEN(TRIM(F101))=0</formula>
+      <formula>LEN(TRIM(F118))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5437,6 +5961,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61906550-8AEF-4C38-94D0-75CC1BE5A7B6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E519CF22-2302-4926-B635-3314F23809F8}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>